<commit_message>
1. adjusted the structure for UMLEvalutor.js. 2. fixed the columns for use case point in model evaluations. 3. fixed the linear estimator for use case point effort estimation model
</commit_message>
<xml_diff>
--- a/data/577 Projects/benchmark/useCaseEvaluationLoad.xlsx
+++ b/data/577 Projects/benchmark/useCaseEvaluationLoad.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="useCaseEvaluationLoad" sheetId="1" r:id="rId1"/>
@@ -731,9 +731,6 @@
     <t>Private Message - Florist</t>
   </si>
   <si>
-    <t>TN</t>
-  </si>
-  <si>
     <t>F14a_mobile_application_for_mobile_controlled_lighting</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>Send Messages to Other Language Learner</t>
+  </si>
+  <si>
+    <t>NT</t>
   </si>
 </sst>
 </file>
@@ -1573,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q12" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -10085,10 +10085,10 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
+        <v>236</v>
+      </c>
+      <c r="C222" t="s">
         <v>237</v>
-      </c>
-      <c r="C222" t="s">
-        <v>238</v>
       </c>
       <c r="D222">
         <v>4</v>
@@ -10124,10 +10124,10 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C223" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D223">
         <v>2</v>
@@ -10163,10 +10163,10 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C224" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D224">
         <v>4</v>
@@ -10202,10 +10202,10 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C225" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D225">
         <v>4</v>
@@ -10241,10 +10241,10 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C226" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D226">
         <v>4</v>
@@ -10280,7 +10280,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C227" t="s">
         <v>12</v>
@@ -10319,7 +10319,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C228" t="s">
         <v>13</v>
@@ -10358,10 +10358,10 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
+        <v>242</v>
+      </c>
+      <c r="C229" t="s">
         <v>243</v>
-      </c>
-      <c r="C229" t="s">
-        <v>244</v>
       </c>
       <c r="D229">
         <v>3</v>
@@ -10397,10 +10397,10 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C230" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D230">
         <v>4</v>
@@ -10436,10 +10436,10 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C231" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D231">
         <v>2</v>
@@ -10475,10 +10475,10 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C232" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D232">
         <v>4</v>
@@ -10518,7 +10518,7 @@
   <dimension ref="A1:L221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10539,7 +10539,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -19032,8 +19032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19054,7 +19054,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -27544,10 +27544,10 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
+        <v>236</v>
+      </c>
+      <c r="C222" t="s">
         <v>237</v>
-      </c>
-      <c r="C222" t="s">
-        <v>238</v>
       </c>
       <c r="D222">
         <v>4</v>
@@ -27583,10 +27583,10 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C223" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D223">
         <v>2</v>
@@ -27622,10 +27622,10 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C224" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D224">
         <v>4</v>
@@ -27661,10 +27661,10 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C225" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D225">
         <v>4</v>
@@ -27700,10 +27700,10 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C226" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D226">
         <v>4</v>
@@ -27739,7 +27739,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C227" t="s">
         <v>12</v>
@@ -27778,7 +27778,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C228" t="s">
         <v>13</v>
@@ -27817,10 +27817,10 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
+        <v>242</v>
+      </c>
+      <c r="C229" t="s">
         <v>243</v>
-      </c>
-      <c r="C229" t="s">
-        <v>244</v>
       </c>
       <c r="D229">
         <v>3</v>
@@ -27856,10 +27856,10 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C230" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D230">
         <v>4</v>
@@ -27895,10 +27895,10 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C231" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D231">
         <v>2</v>
@@ -27934,10 +27934,10 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C232" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D232">
         <v>4</v>

</xml_diff>